<commit_message>
Changed TP to TA where uncertain
</commit_message>
<xml_diff>
--- a/compact_data/Madrid.xlsx
+++ b/compact_data/Madrid.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -124,15 +123,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>TP1</t>
-  </si>
-  <si>
-    <t>TP2</t>
-  </si>
-  <si>
-    <t>TP3</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -150,12 +140,21 @@
   <si>
     <t>Time3</t>
   </si>
+  <si>
+    <t>TA1</t>
+  </si>
+  <si>
+    <t>TA2</t>
+  </si>
+  <si>
+    <t>TA3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -176,6 +175,22 @@
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,8 +219,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -225,7 +242,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -558,7 +577,7 @@
   <dimension ref="A1:L1472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -643,6 +662,9 @@
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
@@ -651,9 +673,6 @@
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
@@ -694,31 +713,31 @@
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -50832,7 +50851,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>